<commit_message>
fix Procfile to worker
</commit_message>
<xml_diff>
--- a/data/senales.xlsx
+++ b/data/senales.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q210"/>
+  <dimension ref="A1:Q211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10701,6 +10701,55 @@
         </is>
       </c>
     </row>
+    <row r="211">
+      <c r="A211" t="inlineStr"/>
+      <c r="B211" t="inlineStr"/>
+      <c r="C211" t="inlineStr"/>
+      <c r="D211" t="inlineStr"/>
+      <c r="E211" t="inlineStr"/>
+      <c r="F211" t="inlineStr"/>
+      <c r="G211" t="inlineStr"/>
+      <c r="H211" t="inlineStr"/>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>EUR/CHF OTC</t>
+        </is>
+      </c>
+      <c r="J211" t="n">
+        <v>1.15426</v>
+      </c>
+      <c r="K211" t="n">
+        <v>4.46</v>
+      </c>
+      <c r="L211" t="inlineStr">
+        <is>
+          <t>🔴 VENDER (SELL)</t>
+        </is>
+      </c>
+      <c r="M211" t="n">
+        <v>93</v>
+      </c>
+      <c r="N211" t="inlineStr">
+        <is>
+          <t>Baja</t>
+        </is>
+      </c>
+      <c r="O211" t="inlineStr">
+        <is>
+          <t>Contexto favorable por velas</t>
+        </is>
+      </c>
+      <c r="P211" t="inlineStr">
+        <is>
+          <t>5m</t>
+        </is>
+      </c>
+      <c r="Q211" t="inlineStr">
+        <is>
+          <t>2025-09-10 22:33:55</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>